<commit_message>
columns name horizontal alignment repair
</commit_message>
<xml_diff>
--- a/src/temp/countries.xlsx
+++ b/src/temp/countries.xlsx
@@ -2039,12 +2039,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>